<commit_message>
Maven project added for recovery sep29/22
</commit_message>
<xml_diff>
--- a/Excel/SampleExcel.xlsx
+++ b/Excel/SampleExcel.xlsx
@@ -4,19 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="84" windowWidth="16260" windowHeight="5856"/>
+    <workbookView xWindow="384" yWindow="84" windowWidth="16260" windowHeight="5856" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Greens" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
     <t>Name</t>
   </si>
@@ -37,9 +36,6 @@
   </si>
   <si>
     <t>Ramesh</t>
-  </si>
-  <si>
-    <t>Eswar</t>
   </si>
   <si>
     <t>Balu</t>
@@ -58,8 +54,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -394,16 +389,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="15.6640625" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="15.21875" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="15.88671875" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="14.77734375" collapsed="false"/>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="15.21875" customWidth="1"/>
+    <col min="3" max="3" width="15.88671875" customWidth="1"/>
+    <col min="4" max="4" width="14.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -450,7 +445,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
@@ -464,7 +459,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
@@ -478,10 +473,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
         <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>10</v>
       </c>
       <c r="C6">
         <v>8968898989</v>
@@ -499,19 +494,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>

</xml_diff>